<commit_message>
3 new EventTrigger Udpate
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/EventResult_Data.xlsx
+++ b/GameDesign/ExcelData/EventResult_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E3F0B4-AAFD-4C12-ACA9-489E2A0C74D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7C6C12-7A64-4B25-A4DC-28CA12C5F1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5508" yWindow="1056" windowWidth="13752" windowHeight="7428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>long</t>
   </si>
@@ -384,10 +384,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dangerous_Mission_2_4_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>To be continue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -411,10 +407,6 @@
     <t>Dangerous_Mission_0_1</t>
   </si>
   <si>
-    <t>Dangerous_Mission_0_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Village_Teenager_Summary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -448,6 +440,18 @@
   </si>
   <si>
     <t>[112,309]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色到了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建造了一个弹药箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色开打</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -809,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -999,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>20</v>
@@ -1019,7 +1023,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>49</v>
@@ -1070,16 +1074,16 @@
         <v>301</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D13" s="4">
         <v>8</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>54</v>
@@ -1242,7 +1246,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="110.4" x14ac:dyDescent="0.25">
@@ -1262,7 +1266,7 @@
         <v>64</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="179.4" x14ac:dyDescent="0.25">
@@ -1310,19 +1314,19 @@
         <v>401</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="4">
         <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="124.2" x14ac:dyDescent="0.25">
@@ -1339,10 +1343,10 @@
         <v>999</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="124.2" x14ac:dyDescent="0.25">
@@ -1359,10 +1363,10 @@
         <v>999</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="69" x14ac:dyDescent="0.25">
@@ -1379,10 +1383,10 @@
         <v>999</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="124.2" x14ac:dyDescent="0.25">
@@ -1399,10 +1403,10 @@
         <v>999</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1410,19 +1414,79 @@
         <v>406</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="D30" s="4">
         <v>999</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>82</v>
+    </row>
+    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>407</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>408</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="4">
+        <v>11</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>409</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="4">
+        <v>12</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>